<commit_message>
tambah kolom jenis kelamin di siswa
</commit_message>
<xml_diff>
--- a/public/file/data_murid_kosong.xlsx
+++ b/public/file/data_murid_kosong.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24729"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\laravel6-admin\public\file\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF98D866-D93A-435D-B5F1-4C8ED9CB8805}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="9870"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>NAMA</t>
   </si>
@@ -35,13 +41,22 @@
   </si>
   <si>
     <t>NIS</t>
+  </si>
+  <si>
+    <t>Jenis Kelamin</t>
+  </si>
+  <si>
+    <t>Pria</t>
+  </si>
+  <si>
+    <t>Wanita</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -68,6 +83,19 @@
       <name val="Arial"/>
       <charset val="134"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -86,15 +114,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
+      <left/>
       <right/>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color auto="1"/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -104,17 +128,21 @@
       <top style="medium">
         <color auto="1"/>
       </top>
-      <bottom style="medium">
-        <color auto="1"/>
+      <bottom style="thin">
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
       <right/>
-      <top/>
-      <bottom style="medium">
+      <top style="medium">
         <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -126,8 +154,8 @@
       <top style="medium">
         <color auto="1"/>
       </top>
-      <bottom style="medium">
-        <color auto="1"/>
+      <bottom style="thin">
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -137,21 +165,9 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -168,6 +184,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -177,6 +209,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -439,269 +474,277 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:G8"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="17.28515625" customWidth="1"/>
     <col min="2" max="2" width="17.7109375" customWidth="1"/>
-    <col min="5" max="5" width="17.85546875" customWidth="1"/>
-    <col min="6" max="6" width="19" customWidth="1"/>
-    <col min="7" max="7" width="20.28515625" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:27">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
-      <c r="M1" s="5"/>
-      <c r="N1" s="5"/>
-      <c r="O1" s="5"/>
-      <c r="P1" s="5"/>
-      <c r="Q1" s="5"/>
-      <c r="R1" s="5"/>
-      <c r="S1" s="5"/>
-      <c r="T1" s="5"/>
-      <c r="U1" s="5"/>
-      <c r="V1" s="5"/>
-      <c r="W1" s="5"/>
-      <c r="X1" s="5"/>
-      <c r="Y1" s="5"/>
-      <c r="Z1" s="5"/>
-      <c r="AA1" s="11"/>
+      <c r="H1" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+      <c r="Q1" s="1"/>
+      <c r="R1" s="1"/>
+      <c r="S1" s="1"/>
+      <c r="T1" s="1"/>
+      <c r="U1" s="1"/>
+      <c r="V1" s="1"/>
+      <c r="W1" s="1"/>
+      <c r="X1" s="1"/>
+      <c r="Y1" s="1"/>
+      <c r="Z1" s="1"/>
+      <c r="AA1" s="7"/>
     </row>
     <row r="2" spans="1:27">
-      <c r="A2" s="6"/>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="8"/>
-      <c r="K2" s="8"/>
-      <c r="L2" s="8"/>
-      <c r="M2" s="9"/>
-      <c r="N2" s="8"/>
-      <c r="O2" s="9"/>
-      <c r="P2" s="8"/>
-      <c r="Q2" s="8"/>
-      <c r="R2" s="8"/>
-      <c r="S2" s="8"/>
-      <c r="T2" s="8"/>
-      <c r="U2" s="8"/>
-      <c r="V2" s="8"/>
-      <c r="W2" s="8"/>
-      <c r="X2" s="8"/>
-      <c r="Y2" s="8"/>
-      <c r="Z2" s="8"/>
-      <c r="AA2" s="11"/>
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="4"/>
+      <c r="O2" s="5"/>
+      <c r="P2" s="4"/>
+      <c r="Q2" s="4"/>
+      <c r="R2" s="4"/>
+      <c r="S2" s="4"/>
+      <c r="T2" s="4"/>
+      <c r="U2" s="4"/>
+      <c r="V2" s="4"/>
+      <c r="W2" s="4"/>
+      <c r="X2" s="4"/>
+      <c r="Y2" s="4"/>
+      <c r="Z2" s="4"/>
+      <c r="AA2" s="7"/>
     </row>
     <row r="3" spans="1:27">
-      <c r="A3" s="6"/>
-      <c r="B3" s="6"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8"/>
-      <c r="K3" s="8"/>
-      <c r="L3" s="8"/>
-      <c r="M3" s="9"/>
-      <c r="N3" s="8"/>
-      <c r="O3" s="9"/>
-      <c r="P3" s="8"/>
-      <c r="Q3" s="10"/>
-      <c r="R3" s="8"/>
-      <c r="S3" s="8"/>
-      <c r="T3" s="8"/>
-      <c r="U3" s="8"/>
-      <c r="V3" s="8"/>
-      <c r="W3" s="8"/>
-      <c r="X3" s="8"/>
-      <c r="Y3" s="8"/>
-      <c r="Z3" s="8"/>
-      <c r="AA3" s="11"/>
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
+      <c r="L3" s="4"/>
+      <c r="M3" s="5"/>
+      <c r="N3" s="4"/>
+      <c r="O3" s="5"/>
+      <c r="P3" s="4"/>
+      <c r="Q3" s="6"/>
+      <c r="R3" s="4"/>
+      <c r="S3" s="4"/>
+      <c r="T3" s="4"/>
+      <c r="U3" s="4"/>
+      <c r="V3" s="4"/>
+      <c r="W3" s="4"/>
+      <c r="X3" s="4"/>
+      <c r="Y3" s="4"/>
+      <c r="Z3" s="4"/>
+      <c r="AA3" s="7"/>
     </row>
     <row r="4" spans="1:27">
-      <c r="A4" s="6"/>
-      <c r="B4" s="6"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="8"/>
-      <c r="I4" s="8"/>
-      <c r="J4" s="8"/>
-      <c r="K4" s="8"/>
-      <c r="L4" s="8"/>
-      <c r="M4" s="9"/>
-      <c r="N4" s="8"/>
-      <c r="O4" s="9"/>
-      <c r="P4" s="8"/>
-      <c r="Q4" s="10"/>
-      <c r="R4" s="8"/>
-      <c r="S4" s="8"/>
-      <c r="T4" s="8"/>
-      <c r="U4" s="8"/>
-      <c r="V4" s="8"/>
-      <c r="W4" s="8"/>
-      <c r="X4" s="8"/>
-      <c r="Y4" s="8"/>
-      <c r="Z4" s="8"/>
-      <c r="AA4" s="11"/>
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4"/>
+      <c r="L4" s="4"/>
+      <c r="M4" s="5"/>
+      <c r="N4" s="4"/>
+      <c r="O4" s="5"/>
+      <c r="P4" s="4"/>
+      <c r="Q4" s="6"/>
+      <c r="R4" s="4"/>
+      <c r="S4" s="4"/>
+      <c r="T4" s="4"/>
+      <c r="U4" s="4"/>
+      <c r="V4" s="4"/>
+      <c r="W4" s="4"/>
+      <c r="X4" s="4"/>
+      <c r="Y4" s="4"/>
+      <c r="Z4" s="4"/>
+      <c r="AA4" s="7"/>
     </row>
     <row r="5" spans="1:27">
-      <c r="A5" s="6"/>
-      <c r="B5" s="6"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="8"/>
-      <c r="I5" s="8"/>
-      <c r="J5" s="8"/>
-      <c r="K5" s="8"/>
-      <c r="L5" s="8"/>
-      <c r="M5" s="9"/>
-      <c r="N5" s="8"/>
-      <c r="O5" s="9"/>
-      <c r="P5" s="8"/>
-      <c r="Q5" s="10"/>
-      <c r="R5" s="8"/>
-      <c r="S5" s="8"/>
-      <c r="T5" s="8"/>
-      <c r="U5" s="8"/>
-      <c r="V5" s="8"/>
-      <c r="W5" s="8"/>
-      <c r="X5" s="8"/>
-      <c r="Y5" s="8"/>
-      <c r="Z5" s="8"/>
-      <c r="AA5" s="11"/>
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
+      <c r="K5" s="4"/>
+      <c r="L5" s="4"/>
+      <c r="M5" s="5"/>
+      <c r="N5" s="4"/>
+      <c r="O5" s="5"/>
+      <c r="P5" s="4"/>
+      <c r="Q5" s="6"/>
+      <c r="R5" s="4"/>
+      <c r="S5" s="4"/>
+      <c r="T5" s="4"/>
+      <c r="U5" s="4"/>
+      <c r="V5" s="4"/>
+      <c r="W5" s="4"/>
+      <c r="X5" s="4"/>
+      <c r="Y5" s="4"/>
+      <c r="Z5" s="4"/>
+      <c r="AA5" s="7"/>
     </row>
     <row r="6" spans="1:27">
-      <c r="A6" s="6"/>
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="8"/>
-      <c r="I6" s="8"/>
-      <c r="J6" s="8"/>
-      <c r="K6" s="8"/>
-      <c r="L6" s="8"/>
-      <c r="M6" s="9"/>
-      <c r="N6" s="8"/>
-      <c r="O6" s="9"/>
-      <c r="P6" s="8"/>
-      <c r="Q6" s="10"/>
-      <c r="R6" s="8"/>
-      <c r="S6" s="8"/>
-      <c r="T6" s="8"/>
-      <c r="U6" s="8"/>
-      <c r="V6" s="8"/>
-      <c r="W6" s="8"/>
-      <c r="X6" s="8"/>
-      <c r="Y6" s="8"/>
-      <c r="Z6" s="8"/>
-      <c r="AA6" s="11"/>
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
+      <c r="J6" s="4"/>
+      <c r="K6" s="4"/>
+      <c r="L6" s="4"/>
+      <c r="M6" s="5"/>
+      <c r="N6" s="4"/>
+      <c r="O6" s="5"/>
+      <c r="P6" s="4"/>
+      <c r="Q6" s="6"/>
+      <c r="R6" s="4"/>
+      <c r="S6" s="4"/>
+      <c r="T6" s="4"/>
+      <c r="U6" s="4"/>
+      <c r="V6" s="4"/>
+      <c r="W6" s="4"/>
+      <c r="X6" s="4"/>
+      <c r="Y6" s="4"/>
+      <c r="Z6" s="4"/>
+      <c r="AA6" s="7"/>
     </row>
     <row r="7" spans="1:27">
-      <c r="A7" s="6"/>
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="8"/>
-      <c r="I7" s="8"/>
-      <c r="J7" s="8"/>
-      <c r="K7" s="8"/>
-      <c r="L7" s="8"/>
-      <c r="M7" s="9"/>
-      <c r="N7" s="8"/>
-      <c r="O7" s="9"/>
-      <c r="P7" s="8"/>
-      <c r="Q7" s="10"/>
-      <c r="R7" s="8"/>
-      <c r="S7" s="8"/>
-      <c r="T7" s="8"/>
-      <c r="U7" s="8"/>
-      <c r="V7" s="8"/>
-      <c r="W7" s="8"/>
-      <c r="X7" s="8"/>
-      <c r="Y7" s="8"/>
-      <c r="Z7" s="8"/>
-      <c r="AA7" s="11"/>
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="4"/>
+      <c r="M7" s="5"/>
+      <c r="N7" s="4"/>
+      <c r="O7" s="5"/>
+      <c r="P7" s="4"/>
+      <c r="Q7" s="6"/>
+      <c r="R7" s="4"/>
+      <c r="S7" s="4"/>
+      <c r="T7" s="4"/>
+      <c r="U7" s="4"/>
+      <c r="V7" s="4"/>
+      <c r="W7" s="4"/>
+      <c r="X7" s="4"/>
+      <c r="Y7" s="4"/>
+      <c r="Z7" s="4"/>
+      <c r="AA7" s="7"/>
     </row>
     <row r="8" spans="1:27">
-      <c r="A8" s="6"/>
-      <c r="B8" s="6"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="8"/>
-      <c r="I8" s="8"/>
-      <c r="J8" s="8"/>
-      <c r="K8" s="8"/>
-      <c r="L8" s="8"/>
-      <c r="M8" s="9"/>
-      <c r="N8" s="8"/>
-      <c r="O8" s="9"/>
-      <c r="P8" s="8"/>
-      <c r="Q8" s="10"/>
-      <c r="R8" s="8"/>
-      <c r="S8" s="8"/>
-      <c r="T8" s="8"/>
-      <c r="U8" s="8"/>
-      <c r="V8" s="8"/>
-      <c r="W8" s="8"/>
-      <c r="X8" s="8"/>
-      <c r="Y8" s="8"/>
-      <c r="Z8" s="8"/>
-      <c r="AA8" s="11"/>
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="4"/>
+      <c r="K8" s="4"/>
+      <c r="L8" s="4"/>
+      <c r="M8" s="5"/>
+      <c r="N8" s="4"/>
+      <c r="O8" s="5"/>
+      <c r="P8" s="4"/>
+      <c r="Q8" s="6"/>
+      <c r="R8" s="4"/>
+      <c r="S8" s="4"/>
+      <c r="T8" s="4"/>
+      <c r="U8" s="4"/>
+      <c r="V8" s="4"/>
+      <c r="W8" s="4"/>
+      <c r="X8" s="4"/>
+      <c r="Y8" s="4"/>
+      <c r="Z8" s="4"/>
+      <c r="AA8" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555596" footer="0.51180555555555596"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>